<commit_message>
tantai: change search feature
</commit_message>
<xml_diff>
--- a/export/exp_danhsach_10072019.xlsx
+++ b/export/exp_danhsach_10072019.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
   <si>
     <t>STT</t>
   </si>
@@ -44,106 +44,169 @@
     <t>Tên ngành</t>
   </si>
   <si>
-    <t>TS1906S1</t>
-  </si>
-  <si>
-    <t>M0619001</t>
-  </si>
-  <si>
-    <t>Lê Quốc Bảo</t>
+    <t>TN1942S1</t>
+  </si>
+  <si>
+    <t>M4219001</t>
+  </si>
+  <si>
+    <t>Lê Hải Bằng</t>
   </si>
   <si>
     <t>Nam</t>
   </si>
   <si>
-    <t>21/01/1984</t>
-  </si>
-  <si>
-    <t>Vĩnh Long</t>
-  </si>
-  <si>
-    <t>Nuôi trồng thủy sản</t>
-  </si>
-  <si>
-    <t>M0619002</t>
-  </si>
-  <si>
-    <t>Lê Tính Cảm</t>
-  </si>
-  <si>
-    <t>02/10/1993</t>
-  </si>
-  <si>
-    <t>Quảng Trị</t>
-  </si>
-  <si>
-    <t>M0619003</t>
-  </si>
-  <si>
-    <t>Trương Quốc Duẩn</t>
-  </si>
-  <si>
-    <t>02/09/1979</t>
+    <t>02/10/1987</t>
+  </si>
+  <si>
+    <t>Đồng Tháp</t>
+  </si>
+  <si>
+    <t>Kỹ thuật xây dựng công trình thủy</t>
+  </si>
+  <si>
+    <t>M4219002</t>
+  </si>
+  <si>
+    <t>Nguyễn Pham Tiến Dũng</t>
+  </si>
+  <si>
+    <t>12/12/1986</t>
+  </si>
+  <si>
+    <t>Cần Thơ</t>
+  </si>
+  <si>
+    <t>M4219003</t>
+  </si>
+  <si>
+    <t>Nguyễn Duy Điệp</t>
+  </si>
+  <si>
+    <t>28/11/1981</t>
+  </si>
+  <si>
+    <t>Vĩnh Phúc</t>
+  </si>
+  <si>
+    <t>M4219004</t>
+  </si>
+  <si>
+    <t>Chau Kim Kha</t>
+  </si>
+  <si>
+    <t>02/02/1981</t>
+  </si>
+  <si>
+    <t>Sóc Trăng</t>
+  </si>
+  <si>
+    <t>M4219005</t>
+  </si>
+  <si>
+    <t>Lê Thị Tuyết Lâm</t>
+  </si>
+  <si>
+    <t>Nữ</t>
+  </si>
+  <si>
+    <t>31/07/1994</t>
   </si>
   <si>
     <t>Cà Mau</t>
   </si>
   <si>
-    <t>M0619004</t>
-  </si>
-  <si>
-    <t>Lê Thị Thùy Dung</t>
-  </si>
-  <si>
-    <t>Nữ</t>
-  </si>
-  <si>
-    <t>26/03/1986</t>
-  </si>
-  <si>
-    <t>Cần Thơ</t>
-  </si>
-  <si>
-    <t>M0619005</t>
-  </si>
-  <si>
-    <t>Mai Thị Yến Duy</t>
-  </si>
-  <si>
-    <t>10/03/1996</t>
+    <t>M4219006</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Kim Loan</t>
+  </si>
+  <si>
+    <t>15/07/1984</t>
+  </si>
+  <si>
+    <t>Hậu Giang</t>
+  </si>
+  <si>
+    <t>M4219007</t>
+  </si>
+  <si>
+    <t>Lưu Thanh Lộng</t>
+  </si>
+  <si>
+    <t>00/00/1985</t>
+  </si>
+  <si>
+    <t>M4219008</t>
+  </si>
+  <si>
+    <t>Nguyễn Khánh Phong</t>
+  </si>
+  <si>
+    <t>31/03/1993</t>
+  </si>
+  <si>
+    <t>M4219009</t>
+  </si>
+  <si>
+    <t>Hồ Trịnh Anh Quân</t>
+  </si>
+  <si>
+    <t>05/10/1983</t>
+  </si>
+  <si>
+    <t>Quảng Nam</t>
+  </si>
+  <si>
+    <t>M4219010</t>
+  </si>
+  <si>
+    <t>Nguyễn Khắc Sơn</t>
+  </si>
+  <si>
+    <t>11/05/1982</t>
+  </si>
+  <si>
+    <t>Hải Phòng</t>
+  </si>
+  <si>
+    <t>M4219011</t>
+  </si>
+  <si>
+    <t>Nguyễn Ngọc Thuận</t>
+  </si>
+  <si>
+    <t>09/06/1993</t>
+  </si>
+  <si>
+    <t>M4219012</t>
+  </si>
+  <si>
+    <t>Trần Xuân Thủy</t>
+  </si>
+  <si>
+    <t>25/09/1989</t>
+  </si>
+  <si>
+    <t>M4219013</t>
+  </si>
+  <si>
+    <t>Phạm Hồng Tiến</t>
+  </si>
+  <si>
+    <t>01/01/1989</t>
   </si>
   <si>
     <t>Trà Vinh</t>
   </si>
   <si>
-    <t>M0619006</t>
-  </si>
-  <si>
-    <t>Phan Thị Hừng</t>
-  </si>
-  <si>
-    <t>06/11/1980</t>
-  </si>
-  <si>
-    <t>M0619007</t>
-  </si>
-  <si>
-    <t>Huỳnh Nguyễn Bình Khang</t>
-  </si>
-  <si>
-    <t>09/12/1986</t>
-  </si>
-  <si>
-    <t>M0619008</t>
-  </si>
-  <si>
-    <t>Châu Khánh Lộc</t>
-  </si>
-  <si>
-    <t>17/10/1984</t>
-  </si>
-  <si>
-    <t>An Giang</t>
+    <t>M4219014</t>
+  </si>
+  <si>
+    <t>Lê Văn Toàn</t>
+  </si>
+  <si>
+    <t>14/05/1990</t>
   </si>
 </sst>
 </file>
@@ -482,7 +545,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,7 +584,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2">
-        <v>1</v>
+        <v>271</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -530,7 +593,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>312</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -550,7 +613,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3">
-        <v>2</v>
+        <v>272</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -559,7 +622,7 @@
         <v>16</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>313</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
@@ -579,7 +642,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -588,7 +651,7 @@
         <v>20</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>314</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
@@ -608,7 +671,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5">
-        <v>4</v>
+        <v>274</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -617,19 +680,19 @@
         <v>24</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>316</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
       </c>
       <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
         <v>26</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>27</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
       </c>
       <c r="I5" t="s">
         <v>15</v>
@@ -637,22 +700,22 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6">
-        <v>5</v>
+        <v>275</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <v>317</v>
+      </c>
+      <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
       </c>
       <c r="G6" t="s">
         <v>31</v>
@@ -666,7 +729,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7">
-        <v>6</v>
+        <v>276</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -675,19 +738,19 @@
         <v>33</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>318</v>
       </c>
       <c r="E7" t="s">
         <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
         <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I7" t="s">
         <v>15</v>
@@ -695,28 +758,28 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8">
+        <v>319</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" t="s">
         <v>36</v>
-      </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" t="s">
-        <v>28</v>
       </c>
       <c r="I8" t="s">
         <v>15</v>
@@ -724,30 +787,204 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9">
-        <v>8</v>
+        <v>278</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9">
-        <v>9</v>
+        <v>320</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="I9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>279</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10">
+        <v>322</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>280</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11">
+        <v>323</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>281</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12">
+        <v>324</v>
+      </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>282</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13">
+        <v>325</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>283</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14">
+        <v>326</v>
+      </c>
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>284</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15">
+        <v>327</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>